<commit_message>
ajustado algumas regras de perfil e papeis dentro da faculdade
</commit_message>
<xml_diff>
--- a/front-end/public/example.xlsx
+++ b/front-end/public/example.xlsx
@@ -34,10 +34,10 @@
     <t>Nome do usuário</t>
   </si>
   <si>
-    <t>administrador/coordenador/usuario</t>
+    <t>[ administrador | servidor | usuario ]</t>
   </si>
   <si>
-    <t>servidor/aluno/externo</t>
+    <t>[ professor | direcao | secretaria | aluno | externo ]</t>
   </si>
 </sst>
 </file>
@@ -54,7 +54,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,7 +75,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -297,7 +298,7 @@
     <col customWidth="1" min="2" max="2" width="27.13"/>
     <col customWidth="1" min="3" max="3" width="17.13"/>
     <col customWidth="1" min="4" max="4" width="29.38"/>
-    <col customWidth="1" min="5" max="5" width="29.25"/>
+    <col customWidth="1" min="5" max="5" width="40.5"/>
     <col customWidth="1" min="6" max="6" width="12.63"/>
   </cols>
   <sheetData>
@@ -319,13 +320,13 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1625,6 +1626,8 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionado algumas configurações para pegar a configuração com base na variavel de ambiente
</commit_message>
<xml_diff>
--- a/front-end/public/example.xlsx
+++ b/front-end/public/example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>E-mail</t>
   </si>
@@ -25,19 +25,13 @@
     <t>Cargo</t>
   </si>
   <si>
-    <t>Papel</t>
-  </si>
-  <si>
     <t>email@email.com</t>
   </si>
   <si>
     <t>Nome do usuário</t>
   </si>
   <si>
-    <t>[ administrador | servidor | usuario ]</t>
-  </si>
-  <si>
-    <t>[ professor | direcao | secretaria | aluno | externo ]</t>
+    <t>[ administrador | servidor | aluno ]</t>
   </si>
 </sst>
 </file>
@@ -315,26 +309,22 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
ajustado o nome da função de reservas, no front e back-end
</commit_message>
<xml_diff>
--- a/front-end/public/example.xlsx
+++ b/front-end/public/example.xlsx
@@ -22,7 +22,7 @@
     <t>Senha</t>
   </si>
   <si>
-    <t>Cargo</t>
+    <t>Perfil</t>
   </si>
   <si>
     <t>email@email.com</t>
@@ -38,12 +38,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -58,18 +63,35 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -309,365 +331,365 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>

</xml_diff>